<commit_message>
ensuring detec. template is updated
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@98264 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136B93AD-3AFE-9045-875F-86839709E8B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B104FDC-DD22-E94B-B78F-BAFD69360311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1480" windowWidth="32720" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,7 +963,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update template for detection data terms
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@98327 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B104FDC-DD22-E94B-B78F-BAFD69360311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EAC718-8513-794C-AEFE-82D82C59FABD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1480" windowWidth="32720" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>variable</t>
   </si>
@@ -53,9 +53,6 @@
     <t>domain</t>
   </si>
   <si>
-    <t>stool</t>
-  </si>
-  <si>
     <t>Bacteria</t>
   </si>
   <si>
@@ -117,6 +114,24 @@
   </si>
   <si>
     <t>&lt;--INPUT | OUTPUT --&gt;</t>
+  </si>
+  <si>
+    <t>website parent</t>
+  </si>
+  <si>
+    <t>website grandparent</t>
+  </si>
+  <si>
+    <t>&lt;--ClinEpi output | ontology output--&gt;</t>
+  </si>
+  <si>
+    <t>Parent term in ClinEpi (which genus in which sample type)</t>
+  </si>
+  <si>
+    <t>blood</t>
+  </si>
+  <si>
+    <t>(which domain in which sample type)</t>
   </si>
 </sst>
 </file>
@@ -960,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,13 +992,13 @@
     <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="23.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="41.83203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="23.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,59 +1015,75 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="J2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -1061,13 +1092,21 @@
         <f>$G3&amp;IF($C3="TAC"," Ct value","")&amp;IF($D3="count"," count","")&amp;", by "&amp;IF($C3="TAC","TAC",$C3)&amp;IF($D3="raw"," result","")</f>
         <v>Shigella flexneri serotype 3A Ct value, by TAC result</v>
       </c>
+      <c r="J3" s="1" t="str">
+        <f>F3&amp;" in "&amp;B3</f>
+        <v>Shigella in blood</v>
+      </c>
       <c r="K3" s="1" t="str">
+        <f>E3&amp; " in "&amp;B3</f>
+        <v>Bacteria in blood</v>
+      </c>
+      <c r="M3" s="1" t="str">
         <f>IF(D3="boolean","presence of",IF(D3="count","count of","data about"))&amp;" "&amp;G3&amp;" by "&amp;C3</f>
         <v>data about Shigella flexneri serotype 3A by TAC</v>
       </c>
-      <c r="L3" s="1" t="str">
+      <c r="N3" s="1" t="str">
         <f>IF($D3="count","a count of the number of ",IF($D3="boolean","a categorical measurement datum","a data item")&amp;" that is about ")&amp;$G3&amp;" and is the specified output of some "&amp;C3&amp;" assay, which achieves an organism identification objective and has as specified input a "&amp;B3&amp;" specimen from an organism"</f>
-        <v>a data item that is about Shigella flexneri serotype 3A and is the specified output of some TAC assay, which achieves an organism identification objective and has as specified input a stool specimen from an organism</v>
+        <v>a data item that is about Shigella flexneri serotype 3A and is the specified output of some TAC assay, which achieves an organism identification objective and has as specified input a blood specimen from an organism</v>
       </c>
     </row>
   </sheetData>
@@ -1090,29 +1129,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1120,12 +1159,12 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added value col to detection template
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@98454 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC00254-53B0-A243-AFD1-91DCF6CAFCC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C05DC50-0B87-D94B-9185-636ADA80D3C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1480" windowWidth="32720" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>variable</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Ct value</t>
-  </si>
-  <si>
-    <t>^^^ fix this for Ct !!! ^^^</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1001,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1129,7 +1126,7 @@
         <v>34</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f>$H3&amp;IF(AND($C3="TAC",$D3="raw")," Ct value","")&amp;IF($D3="count"," count","")&amp;", by "&amp;IF($C3="TAC","TAC",$C3)&amp;IF($D3="raw"," result","")</f>
+        <f>$H3&amp;IF($D3="raw",IF($E3&lt;&gt;""," ","")&amp;$E3,"")&amp;IF($D3="count"," count","")&amp;", by "&amp;IF($C3="TAC","TAC",$C3)&amp;IF($D3="raw"," result","")</f>
         <v>Adenovirus Ct value, by TAC result</v>
       </c>
       <c r="K3" s="1" t="str">
@@ -1153,10 +1150,8 @@
         <v>('data item' and is about some Adenovirus) and is_specified_output_of some (('TAC assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen from organism')</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="J5" s="2" t="s">
-        <v>41</v>
-      </c>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed truncations of 'Nalidixic'
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@98992 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0832E16-266D-8445-AE67-1E78EC95F8D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB87D81-6B08-6443-AACF-939D20C5018F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1480" windowWidth="32720" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>variable</t>
   </si>
@@ -68,24 +68,12 @@
     <t>PCR</t>
   </si>
   <si>
-    <t>IRI</t>
-  </si>
-  <si>
     <t>ClinEpi</t>
   </si>
   <si>
-    <t>ontology</t>
-  </si>
-  <si>
-    <t>fluorogenic PCR assay</t>
-  </si>
-  <si>
     <t>PCR assay</t>
   </si>
   <si>
-    <t>bacteriology assay</t>
-  </si>
-  <si>
     <t>culture</t>
   </si>
   <si>
@@ -147,6 +135,24 @@
   </si>
   <si>
     <t>(Ontology output section still under construction)</t>
+  </si>
+  <si>
+    <t>TaqMan</t>
+  </si>
+  <si>
+    <t>an assay, of which a polymerase chain reaction is part,</t>
+  </si>
+  <si>
+    <t>bacteriological assay</t>
+  </si>
+  <si>
+    <t>a bacteriological assay</t>
+  </si>
+  <si>
+    <t>a fluorogenic PCR assay</t>
+  </si>
+  <si>
+    <t>assay and 'has part' some 'polymerase chain reaction'</t>
   </si>
 </sst>
 </file>
@@ -638,7 +644,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -646,6 +652,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1001,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,7 +1047,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -1052,19 +1059,19 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
@@ -1073,72 +1080,72 @@
         <v>7</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="str">
         <f>$H3&amp;IF($D3="raw",IF($E3&lt;&gt;""," ","")&amp;$E3,"")&amp;IF($D3="count"," count","")&amp;", by "&amp;IF($C3="TAC","TAC",$C3)&amp;IF($D3="raw"," result","")</f>
-        <v>Adenovirus Ct value, by TAC result</v>
+        <v>Adenovirus Ct value, by culture result</v>
       </c>
       <c r="K3" s="1" t="str">
         <f>IF($D3="raw","Raw "&amp;LOWER($F3)&amp;" data",IF($G3="",$H3,$G3)&amp;" in "&amp;$B3)</f>
@@ -1149,20 +1156,26 @@
         <v>Raw test result</v>
       </c>
       <c r="N3" s="1" t="str">
-        <f>IF(D3="boolean","presence of",IF(D3="count","count of","data about"))&amp;" "&amp;H3&amp;" by "&amp;C3</f>
-        <v>data about Adenovirus by TAC</v>
+        <f>IF(D3="boolean","presence of",IF(D3="count","count of","data about"))&amp;" "&amp;H3&amp;" by "&amp;IF(ISNA(VLOOKUP(C3,lookup!A2:B4,2)=TRUE),C3,VLOOKUP(C3,lookup!A2:B4,2))</f>
+        <v>data about Adenovirus by bacteriology</v>
       </c>
       <c r="O3" s="1" t="str">
         <f>IF($D3="count","a count of the number of ",IF($D3="boolean","a categorical measurement datum","a data item")&amp;" that is about ")&amp;$H3&amp;" and is the specified output of some "&amp;$C3&amp;" assay, which achieves an organism identification objective and has as specified input a "&amp;$B3&amp;" specimen from an organism"</f>
-        <v>a data item that is about Adenovirus and is the specified output of some TAC assay, which achieves an organism identification objective and has as specified input a stool specimen from an organism</v>
+        <v>a data item that is about Adenovirus and is the specified output of some culture assay, which achieves an organism identification objective and has as specified input a stool specimen from an organism</v>
       </c>
       <c r="P3" s="1" t="str">
         <f>"("&amp;IF($D3="count","count and",IF($D3="boolean","'categorical measurement datum' and","'data item' and")&amp;" is about some ")&amp;$H3&amp;") and is_specified_output_of some (('"&amp;$C3&amp;" assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B3&amp;" specimen from organism')"</f>
-        <v>('data item' and is about some Adenovirus) and is_specified_output_of some (('TAC assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen from organism')</v>
+        <v>('data item' and is about some Adenovirus) and is_specified_output_of some (('culture assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen from organism')</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M6" s="1" t="e">
+        <f>VLOOKUP(A3,lookup!A2:B4,2)</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1171,58 +1184,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AA4B01-1A62-8B4E-8367-99824A1C2D4E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>"'fluorogenic PCR assay'"</f>
+        <v>'fluorogenic PCR assay'</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D6">
+    <sortCondition ref="A2:A6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed detection template example
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@99028 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB87D81-6B08-6443-AACF-939D20C5018F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23081DDE-884C-1C4E-AA76-FE57AAC6D212}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1480" windowWidth="32720" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="detection_template_csv" sheetId="1" r:id="rId1"/>
-    <sheet name="lookup" sheetId="2" r:id="rId2"/>
+    <sheet name="antibiotics" sheetId="3" r:id="rId2"/>
+    <sheet name="lookup" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>variable</t>
   </si>
@@ -59,12 +60,6 @@
     <t>Shigella</t>
   </si>
   <si>
-    <t>TAC</t>
-  </si>
-  <si>
-    <t>raw</t>
-  </si>
-  <si>
     <t>PCR</t>
   </si>
   <si>
@@ -74,9 +69,6 @@
     <t>PCR assay</t>
   </si>
   <si>
-    <t>culture</t>
-  </si>
-  <si>
     <t>Enter assay according to how it should appear in the label: bacteriology, TAQ, ELISA, …</t>
   </si>
   <si>
@@ -113,12 +105,6 @@
     <t>(which domain in which sample type)</t>
   </si>
   <si>
-    <t>Adenovirus</t>
-  </si>
-  <si>
-    <t>Virus</t>
-  </si>
-  <si>
     <t>axiom</t>
   </si>
   <si>
@@ -153,6 +139,33 @@
   </si>
   <si>
     <t>assay and 'has part' some 'polymerase chain reaction'</t>
+  </si>
+  <si>
+    <t>TAQ</t>
+  </si>
+  <si>
+    <t>antibiotic</t>
+  </si>
+  <si>
+    <t>treatment or medication</t>
+  </si>
+  <si>
+    <t>clinical visit?</t>
+  </si>
+  <si>
+    <t>control?</t>
+  </si>
+  <si>
+    <t>enrollment?</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>Shigella dysenteriae serotype 1</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -1008,26 +1021,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.33203125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="23.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="41.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="34.83203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="23.83203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="32.83203125" customWidth="1"/>
     <col min="16" max="16" width="33.83203125" customWidth="1"/>
@@ -1037,7 +1051,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1047,7 +1061,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -1059,19 +1073,19 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
@@ -1080,102 +1094,96 @@
         <v>7</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="102" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>33</v>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="J3" s="1" t="str">
         <f>$H3&amp;IF($D3="raw",IF($E3&lt;&gt;""," ","")&amp;$E3,"")&amp;IF($D3="count"," count","")&amp;", by "&amp;IF($C3="TAC","TAC",$C3)&amp;IF($D3="raw"," result","")</f>
-        <v>Adenovirus Ct value, by culture result</v>
+        <v>Shigella dysenteriae serotype 1, by bacteriology</v>
       </c>
       <c r="K3" s="1" t="str">
         <f>IF($D3="raw","Raw "&amp;LOWER($F3)&amp;" data",IF($G3="",$H3,$G3)&amp;" in "&amp;$B3)</f>
-        <v>Raw virus data</v>
+        <v>Shigella in stool</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>IF($D3="raw","Raw test result",$F3&amp; " in "&amp;$B3)</f>
-        <v>Raw test result</v>
+        <v>Bacteria in stool</v>
       </c>
       <c r="N3" s="1" t="str">
-        <f>IF(D3="boolean","presence of",IF(D3="count","count of","data about"))&amp;" "&amp;H3&amp;" by "&amp;IF(ISNA(VLOOKUP(C3,lookup!A2:B4,2)=TRUE),C3,VLOOKUP(C3,lookup!A2:B4,2))</f>
-        <v>data about Adenovirus by bacteriology</v>
+        <f>IF(D3="boolean","presence of",IF(D3="count","count of","data about"))&amp;" "&amp;H3&amp;" by "&amp;IF(ISNA(VLOOKUP(C3,lookup!A2:B4,2,FALSE)=TRUE),C3,VLOOKUP(C3,lookup!A2:B4,2))</f>
+        <v>presence of Shigella dysenteriae serotype 1 by bacteriology</v>
       </c>
       <c r="O3" s="1" t="str">
         <f>IF($D3="count","a count of the number of ",IF($D3="boolean","a categorical measurement datum","a data item")&amp;" that is about ")&amp;$H3&amp;" and is the specified output of some "&amp;$C3&amp;" assay, which achieves an organism identification objective and has as specified input a "&amp;$B3&amp;" specimen from an organism"</f>
-        <v>a data item that is about Adenovirus and is the specified output of some culture assay, which achieves an organism identification objective and has as specified input a stool specimen from an organism</v>
+        <v>a categorical measurement datum that is about Shigella dysenteriae serotype 1 and is the specified output of some bacteriology assay, which achieves an organism identification objective and has as specified input a stool specimen from an organism</v>
       </c>
       <c r="P3" s="1" t="str">
         <f>"("&amp;IF($D3="count","count and",IF($D3="boolean","'categorical measurement datum' and","'data item' and")&amp;" is about some ")&amp;$H3&amp;") and is_specified_output_of some (('"&amp;$C3&amp;" assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B3&amp;" specimen from organism')"</f>
-        <v>('data item' and is about some Adenovirus) and is_specified_output_of some (('culture assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen from organism')</v>
+        <v>('categorical measurement datum' and is about some Shigella dysenteriae serotype 1) and is_specified_output_of some (('bacteriology assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen from organism')</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="M6" s="1" t="e">
-        <f>VLOOKUP(A3,lookup!A2:B4,2)</f>
-        <v>#N/A</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1183,11 +1191,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0DB369-D91D-804D-8D4A-F6F9B2BC7AF1}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AA4B01-1A62-8B4E-8367-99824A1C2D4E}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1198,7 +1242,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -1207,7 +1251,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1218,35 +1262,35 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3" t="str">
         <f>"'fluorogenic PCR assay'"</f>

</xml_diff>

<commit_message>
changes to MALED based on detection template
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@100333 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F81055-AF1B-9347-811B-A17A20FE4C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14976DB0-E7DF-2240-8C01-C9850DA423AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="1480" windowWidth="32720" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1174,12 +1174,12 @@
         <v>presence of Vibrio cholerae by differential medium assay</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f>IF($D3="count","a count of the number of ",IF($D3="boolean","a categorical measurement datum","a data item")&amp;" that is about ")&amp;$H3&amp;" and is the specified output of some "&amp;$C3&amp;" assay, which achieves an organism identification objective and has as specified input a "&amp;$B3&amp;" specimen from an organism"</f>
-        <v>a categorical measurement datum that is about Vibrio cholerae and is the specified output of some bacteriology assay, which achieves an organism identification objective and has as specified input a stool specimen from an organism</v>
+        <f>IF($D3="count","a count of the number of ",IF($D3="boolean","a categorical measurement datum","a data item")&amp;" that is about ")&amp;$H3&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C3,lookup!A2:B4,2,FALSE)=TRUE),C3,VLOOKUP(C3,lookup!A2:B4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B3&amp;" specimen"</f>
+        <v>a categorical measurement datum that is about Vibrio cholerae and is the specified output of some differential medium assay, which achieves an organism identification objective and has as specified input a stool specimen</v>
       </c>
       <c r="P3" s="1" t="str">
-        <f>"("&amp;IF($D3="count","count and",IF($D3="boolean","'categorical measurement datum' and","'data item' and")&amp;" 'is about' some ")&amp;"'"&amp;$H3&amp;"') and is_specified_output_of some (('"&amp;$C3&amp;" assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B3&amp;" specimen from organism')"</f>
-        <v>('categorical measurement datum' and 'is about' some 'Vibrio cholerae') and is_specified_output_of some (('bacteriology assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen from organism')</v>
+        <f>"("&amp;IF($D3="count","count and",IF($D3="boolean","'categorical measurement datum' and","'data item' and")&amp;" 'is about' some ")&amp;"'"&amp;$H3&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C3,lookup!A2:B4,2,FALSE)=TRUE),C3,VLOOKUP(C3,lookup!A2:B4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B3&amp;" specimen')"</f>
+        <v>('categorical measurement datum' and 'is about' some 'Vibrio cholerae') and is_specified_output_of some (('differential medium assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes to MALED phase 3
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@100848 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444925F9-335F-FE48-A41E-74250AAFA21E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E31C37C-24F2-F047-84FA-8A9FAEA2ECC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1420" windowWidth="32720" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="detection_template_csv" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>variable</t>
   </si>
@@ -67,9 +67,6 @@
     <t>PCR assay</t>
   </si>
   <si>
-    <t>Enter assay according to how it should appear in the label: bacteriology, TAQ, ELISA, …</t>
-  </si>
-  <si>
     <t>Genus or most specified taxonomic rank</t>
   </si>
   <si>
@@ -166,45 +163,6 @@
     <t xml:space="preserve">Ancylostoma </t>
   </si>
   <si>
-    <t xml:space="preserve">Ascaris </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Astrovirus </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blastocystis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campylobacter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clostridium difficile </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cryptosporidium </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entamoeba </t>
-  </si>
-  <si>
-    <t>Bacteriodes</t>
-  </si>
-  <si>
-    <t>Hymenolepis</t>
-  </si>
-  <si>
-    <t>Mycobacterium</t>
-  </si>
-  <si>
-    <t>Norovirus</t>
-  </si>
-  <si>
-    <t>Plesiomonas</t>
-  </si>
-  <si>
-    <t>Schistosoma</t>
-  </si>
-  <si>
     <t>Virus</t>
   </si>
   <si>
@@ -217,39 +175,6 @@
     <t>fluorogenic PCR assay</t>
   </si>
   <si>
-    <t>Blastocystis</t>
-  </si>
-  <si>
-    <t>Campylobacter</t>
-  </si>
-  <si>
-    <t>Clostridium difficile</t>
-  </si>
-  <si>
-    <t>Cryptosporidium</t>
-  </si>
-  <si>
-    <t>Entamoeba</t>
-  </si>
-  <si>
-    <t>Hymenolepis nana</t>
-  </si>
-  <si>
-    <t>Mycobacterium tuberculosis</t>
-  </si>
-  <si>
-    <t>Norovirus GI 1</t>
-  </si>
-  <si>
-    <t>Norovirus GII 4</t>
-  </si>
-  <si>
-    <t>Bacteriodes fragilis</t>
-  </si>
-  <si>
-    <t>Astrovirus</t>
-  </si>
-  <si>
     <t>Adenovirus</t>
   </si>
   <si>
@@ -259,16 +184,16 @@
     <t>Ancylostoma</t>
   </si>
   <si>
-    <t>Ascaris</t>
-  </si>
-  <si>
     <t>input "boolean", "raw", "count", or "aggregate"</t>
   </si>
   <si>
     <t>aggregate</t>
   </si>
   <si>
-    <t>e.g. Ct value, stools</t>
+    <t>e.g. Ct value, stools, 1st monthly stools</t>
+  </si>
+  <si>
+    <t>Enter assay according to how it should appear in the label: bacteriology, TAQ, ELISA, … . Leave blank for MALED aggregate data.</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1041,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -1165,19 +1090,19 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
@@ -1186,73 +1111,82 @@
         <v>7</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
         <v>39</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
       <c r="J3" s="1" t="str">
-        <f>$H3&amp;IF($D3="raw",IF($E3&lt;&gt;""," ","")&amp;$E3,"")&amp;IF($D3="count"," count","")&amp;", by "&amp;IF($C3="TAC","TAC",$C3)&amp;IF($D3="raw"," result","")</f>
+        <f>IF(ISNUMBER(SEARCH("stools",$E3)),"Cumulative sum ","")
+&amp;$H3
+&amp;IF(ISNUMBER(SEARCH("stools",$E3)),"-pos ","")
+&amp;IF(ISNUMBER(SEARCH("1st monthly",$E3)),"1st monthly ","")
+&amp;IF(ISNUMBER(SEARCH("1st diarrheal",$E3)),"1st diarrheal ","")
+&amp;IF(ISNUMBER(SEARCH("stools",$E3)),"stools","")
+&amp;IF($D3="raw",IF($E3&lt;&gt;""," ","")&amp;$E3,"")
+&amp;IF($D3="count"," count","")
+&amp;IF($C3&lt;&gt;"",", by "&amp;$C3,"")
+&amp;IF($D3="raw"," result","")</f>
         <v>Vibrio cholerae, by bacteriology</v>
       </c>
       <c r="K3" s="1" t="str">
-        <f>IF($D3="raw","Raw "&amp;LOWER($F3)&amp;" data",IF($G3="",$H3,$G3)&amp;" in "&amp;$B3)&amp;IF($D3="aggregate"," detection aggregate data","")</f>
-        <v>Vibrio in stool detection aggregate data</v>
+        <f>IF($D3="raw","Raw "&amp;LOWER($F3)&amp;" data",IF($G3="",$H3,IF($D3="aggregate",$H3&amp;" aggregate data",$G3))&amp;" in "&amp;$B3)</f>
+        <v>Vibrio cholerae aggregate data in stool</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>IF($D3="raw","Raw test result",$F3&amp; " in "&amp;$B3)&amp;IF($D3="aggregate"," detection aggregate data","")</f>
@@ -1271,79 +1205,94 @@
         <v>('data item' and 'is about' some 'Vibrio cholerae') and is_specified_output_of some (('differential medium assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f t="shared" ref="J4:J21" si="0">$H4&amp;IF($D4="raw",IF($E4&lt;&gt;""," ","")&amp;$E4,"")&amp;IF($D4="count"," count","")&amp;", by "&amp;IF($C4="TAC","TAC",$C4)&amp;IF($D4="raw"," result","")</f>
-        <v>Adenovirus Ct value, by TAQ result</v>
+        <f>IF(ISNUMBER(SEARCH("stools",$E4)),"Cumulative sum ","")
+&amp;$H4
+&amp;IF(ISNUMBER(SEARCH("stools",$E4)),"-pos ","")
+&amp;IF(ISNUMBER(SEARCH("1st monthly",$E4)),"1st monthly ","")
+&amp;IF(ISNUMBER(SEARCH("1st diarrheal",$E4)),"1st diarrheal ","")
+&amp;IF(ISNUMBER(SEARCH("stools",$E4)),"stools","")
+&amp;IF($D4="raw",IF($E4&lt;&gt;""," ","")&amp;$E4,"")
+&amp;IF($D4="count"," count","")
+&amp;IF($C4&lt;&gt;"",", by "&amp;$C4,"")
+&amp;IF($D4="raw"," result","")</f>
+        <v>Adenovirus, by TAQ result</v>
       </c>
       <c r="K4" s="1" t="str">
-        <f t="shared" ref="K4:K21" si="1">IF($D4="raw","Raw "&amp;LOWER($F4)&amp;" data",IF($G4="",$H4,$G4)&amp;" in "&amp;$B4)</f>
+        <f t="shared" ref="K4:K21" si="0">IF($D4="raw","Raw "&amp;LOWER($F4)&amp;" data",IF($G4="",$H4,$G4)&amp;" in "&amp;$B4)</f>
         <v>Raw virus data</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f t="shared" ref="L4:L21" si="2">IF($D4="raw","Raw test result",$F4&amp; " in "&amp;$B4)</f>
+        <f t="shared" ref="L4:L21" si="1">IF($D4="raw","Raw test result",$F4&amp; " in "&amp;$B4)</f>
         <v>Raw test result</v>
       </c>
       <c r="N4" s="1" t="str">
         <f>IF(D4="boolean","presence of",IF(D4="count","count of",IF(E4="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H4&amp;" by "&amp;IF(ISNA(VLOOKUP(C4,lookup!$A$2:$B$4,2,FALSE)=TRUE),C4,VLOOKUP(C4,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Adenovirus by fluorogenic PCR assay</v>
+        <v>data about Adenovirus by fluorogenic PCR assay</v>
       </c>
       <c r="O4" s="1" t="str">
         <f>IF($D4="count","a count of the number of ",IF($D4="boolean","a categorical measurement datum",IF($E4="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H4&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C4,lookup!$A$2:$B$4,2,FALSE)=TRUE),C4,VLOOKUP(C4,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B4&amp;" specimen")</f>
-        <v>a threshold cycle that is about Adenovirus and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about Adenovirus and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P4" s="1" t="str">
         <f>"("&amp;IF($D4="count","count and",IF($D4="boolean","'categorical measurement datum' and",IF($E4="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H4&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C4,lookup!$A$2:$B$4,2,FALSE)=TRUE),C4,VLOOKUP(C4,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B4&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Adenovirus') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+        <v>('data item' and 'is about' some 'Adenovirus') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="J5" s="1" t="str">
+        <f>IF(ISNUMBER(SEARCH("stools",$E5)),"Cumulative sum ","")
+&amp;$H5
+&amp;IF(ISNUMBER(SEARCH("stools",$E5)),"-pos ","")
+&amp;IF(ISNUMBER(SEARCH("1st monthly",$E5)),"1st monthly ","")
+&amp;IF(ISNUMBER(SEARCH("1st diarrheal",$E5)),"1st diarrheal ","")
+&amp;IF(ISNUMBER(SEARCH("stools",$E5)),"stools","")
+&amp;IF($D5="raw",IF($E5&lt;&gt;""," ","")&amp;$E5,"")
+&amp;IF($D5="count"," count","")
+&amp;IF($C5&lt;&gt;"",", by "&amp;$C5,"")
+&amp;IF($D5="raw"," result","")</f>
+        <v>Aeromonas Ct value, by TAQ result</v>
+      </c>
+      <c r="K5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Aeromonas Ct value, by TAQ result</v>
-      </c>
-      <c r="K5" s="1" t="str">
+        <v>Raw virus data</v>
+      </c>
+      <c r="L5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Raw virus data</v>
-      </c>
-      <c r="L5" s="1" t="str">
-        <f t="shared" si="2"/>
         <v>Raw test result</v>
       </c>
       <c r="N5" s="1" t="str">
@@ -1361,33 +1310,42 @@
     </row>
     <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="J6" s="1" t="str">
+        <f>IF(ISNUMBER(SEARCH("stools",$E6)),"Cumulative sum ","")
+&amp;$H6
+&amp;IF(ISNUMBER(SEARCH("stools",$E6)),"-pos ","")
+&amp;IF(ISNUMBER(SEARCH("1st monthly",$E6)),"1st monthly ","")
+&amp;IF(ISNUMBER(SEARCH("1st diarrheal",$E6)),"1st diarrheal ","")
+&amp;IF(ISNUMBER(SEARCH("stools",$E6)),"stools","")
+&amp;IF($D6="raw",IF($E6&lt;&gt;""," ","")&amp;$E6,"")
+&amp;IF($D6="count"," count","")
+&amp;IF($C6&lt;&gt;"",", by "&amp;$C6,"")
+&amp;IF($D6="raw"," result","")</f>
+        <v>Ancylostoma Ct value, by TAQ result</v>
+      </c>
+      <c r="K6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Ancylostoma Ct value, by TAQ result</v>
-      </c>
-      <c r="K6" s="1" t="str">
+        <v>Raw eukaryota data</v>
+      </c>
+      <c r="L6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Raw eukaryota data</v>
-      </c>
-      <c r="L6" s="1" t="str">
-        <f t="shared" si="2"/>
         <v>Raw test result</v>
       </c>
       <c r="N6" s="1" t="str">
@@ -1403,664 +1361,214 @@
         <v>('threshold cycle' and 'is about' some 'Ancylostoma') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Ascaris Ct value, by TAQ result</v>
-      </c>
-      <c r="K7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw eukaryota data</v>
-      </c>
-      <c r="L7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N7" s="1" t="str">
         <f>IF(D7="boolean","presence of",IF(D7="count","count of",IF(E7="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H7&amp;" by "&amp;IF(ISNA(VLOOKUP(C7,lookup!$A$2:$B$4,2,FALSE)=TRUE),C7,VLOOKUP(C7,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Ascaris by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O7" s="1" t="str">
         <f>IF($D7="count","a count of the number of ",IF($D7="boolean","a categorical measurement datum",IF($E7="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H7&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C7,lookup!$A$2:$B$4,2,FALSE)=TRUE),C7,VLOOKUP(C7,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B7&amp;" specimen")</f>
-        <v>a threshold cycle that is about Ascaris and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P7" s="1" t="str">
         <f>"("&amp;IF($D7="count","count and",IF($D7="boolean","'categorical measurement datum' and",IF($E7="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H7&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C7,lookup!$A$2:$B$4,2,FALSE)=TRUE),C7,VLOOKUP(C7,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B7&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Ascaris') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Astrovirus Ct value, by TAQ result</v>
-      </c>
-      <c r="K8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw virus data</v>
-      </c>
-      <c r="L8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N8" s="1" t="str">
         <f>IF(D8="boolean","presence of",IF(D8="count","count of",IF(E8="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H8&amp;" by "&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Astrovirus by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O8" s="1" t="str">
         <f>IF($D8="count","a count of the number of ",IF($D8="boolean","a categorical measurement datum",IF($E8="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H8&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B8&amp;" specimen")</f>
-        <v>a threshold cycle that is about Astrovirus and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P8" s="1" t="str">
         <f>"("&amp;IF($D8="count","count and",IF($D8="boolean","'categorical measurement datum' and",IF($E8="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H8&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B8&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Astrovirus') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Bacteriodes fragilis Ct value, by TAQ result</v>
-      </c>
-      <c r="K9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw bacteria data</v>
-      </c>
-      <c r="L9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N9" s="1" t="str">
         <f>IF(D9="boolean","presence of",IF(D9="count","count of",IF(E9="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H9&amp;" by "&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Bacteriodes fragilis by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O9" s="1" t="str">
         <f>IF($D9="count","a count of the number of ",IF($D9="boolean","a categorical measurement datum",IF($E9="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H9&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B9&amp;" specimen")</f>
-        <v>a threshold cycle that is about Bacteriodes fragilis and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P9" s="1" t="str">
         <f>"("&amp;IF($D9="count","count and",IF($D9="boolean","'categorical measurement datum' and",IF($E9="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H9&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B9&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Bacteriodes fragilis') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Blastocystis Ct value, by TAQ result</v>
-      </c>
-      <c r="K10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw eukaryota data</v>
-      </c>
-      <c r="L10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N10" s="1" t="str">
         <f>IF(D10="boolean","presence of",IF(D10="count","count of",IF(E10="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H10&amp;" by "&amp;IF(ISNA(VLOOKUP(C10,lookup!$A$2:$B$4,2,FALSE)=TRUE),C10,VLOOKUP(C10,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Blastocystis by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O10" s="1" t="str">
         <f>IF($D10="count","a count of the number of ",IF($D10="boolean","a categorical measurement datum",IF($E10="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H10&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C10,lookup!$A$2:$B$4,2,FALSE)=TRUE),C10,VLOOKUP(C10,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B10&amp;" specimen")</f>
-        <v>a threshold cycle that is about Blastocystis and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P10" s="1" t="str">
         <f>"("&amp;IF($D10="count","count and",IF($D10="boolean","'categorical measurement datum' and",IF($E10="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H10&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C10,lookup!$A$2:$B$4,2,FALSE)=TRUE),C10,VLOOKUP(C10,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B10&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Blastocystis') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Campylobacter Ct value, by TAQ result</v>
-      </c>
-      <c r="K11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw bacteria data</v>
-      </c>
-      <c r="L11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N11" s="1" t="str">
         <f>IF(D11="boolean","presence of",IF(D11="count","count of",IF(E11="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H11&amp;" by "&amp;IF(ISNA(VLOOKUP(C11,lookup!$A$2:$B$4,2,FALSE)=TRUE),C11,VLOOKUP(C11,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Campylobacter by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O11" s="1" t="str">
         <f>IF($D11="count","a count of the number of ",IF($D11="boolean","a categorical measurement datum",IF($E11="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H11&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C11,lookup!$A$2:$B$4,2,FALSE)=TRUE),C11,VLOOKUP(C11,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B11&amp;" specimen")</f>
-        <v>a threshold cycle that is about Campylobacter and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P11" s="1" t="str">
         <f>"("&amp;IF($D11="count","count and",IF($D11="boolean","'categorical measurement datum' and",IF($E11="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H11&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C11,lookup!$A$2:$B$4,2,FALSE)=TRUE),C11,VLOOKUP(C11,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B11&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Campylobacter') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Clostridium difficile Ct value, by TAQ result</v>
-      </c>
-      <c r="K12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw bacteria data</v>
-      </c>
-      <c r="L12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N12" s="1" t="str">
         <f>IF(D12="boolean","presence of",IF(D12="count","count of",IF(E12="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H12&amp;" by "&amp;IF(ISNA(VLOOKUP(C12,lookup!$A$2:$B$4,2,FALSE)=TRUE),C12,VLOOKUP(C12,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Clostridium difficile by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O12" s="1" t="str">
         <f>IF($D12="count","a count of the number of ",IF($D12="boolean","a categorical measurement datum",IF($E12="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H12&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C12,lookup!$A$2:$B$4,2,FALSE)=TRUE),C12,VLOOKUP(C12,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B12&amp;" specimen")</f>
-        <v>a threshold cycle that is about Clostridium difficile and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P12" s="1" t="str">
         <f>"("&amp;IF($D12="count","count and",IF($D12="boolean","'categorical measurement datum' and",IF($E12="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H12&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C12,lookup!$A$2:$B$4,2,FALSE)=TRUE),C12,VLOOKUP(C12,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B12&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Clostridium difficile') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Cryptosporidium Ct value, by TAQ result</v>
-      </c>
-      <c r="K13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw eukaryota data</v>
-      </c>
-      <c r="L13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N13" s="1" t="str">
         <f>IF(D13="boolean","presence of",IF(D13="count","count of",IF(E13="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H13&amp;" by "&amp;IF(ISNA(VLOOKUP(C13,lookup!$A$2:$B$4,2,FALSE)=TRUE),C13,VLOOKUP(C13,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Cryptosporidium by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O13" s="1" t="str">
         <f>IF($D13="count","a count of the number of ",IF($D13="boolean","a categorical measurement datum",IF($E13="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H13&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C13,lookup!$A$2:$B$4,2,FALSE)=TRUE),C13,VLOOKUP(C13,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B13&amp;" specimen")</f>
-        <v>a threshold cycle that is about Cryptosporidium and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P13" s="1" t="str">
         <f>"("&amp;IF($D13="count","count and",IF($D13="boolean","'categorical measurement datum' and",IF($E13="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H13&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C13,lookup!$A$2:$B$4,2,FALSE)=TRUE),C13,VLOOKUP(C13,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B13&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Cryptosporidium') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" t="s">
-        <v>68</v>
-      </c>
-      <c r="J14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Entamoeba Ct value, by TAQ result</v>
-      </c>
-      <c r="K14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw eukaryota data</v>
-      </c>
-      <c r="L14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N14" s="1" t="str">
         <f>IF(D14="boolean","presence of",IF(D14="count","count of",IF(E14="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H14&amp;" by "&amp;IF(ISNA(VLOOKUP(C14,lookup!$A$2:$B$4,2,FALSE)=TRUE),C14,VLOOKUP(C14,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Entamoeba by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O14" s="1" t="str">
         <f>IF($D14="count","a count of the number of ",IF($D14="boolean","a categorical measurement datum",IF($E14="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H14&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C14,lookup!$A$2:$B$4,2,FALSE)=TRUE),C14,VLOOKUP(C14,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B14&amp;" specimen")</f>
-        <v>a threshold cycle that is about Entamoeba and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P14" s="1" t="str">
         <f>"("&amp;IF($D14="count","count and",IF($D14="boolean","'categorical measurement datum' and",IF($E14="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H14&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C14,lookup!$A$2:$B$4,2,FALSE)=TRUE),C14,VLOOKUP(C14,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B14&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Entamoeba') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Hymenolepis nana Ct value, by TAQ result</v>
-      </c>
-      <c r="K15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw eukaryota data</v>
-      </c>
-      <c r="L15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N15" s="1" t="str">
         <f>IF(D15="boolean","presence of",IF(D15="count","count of",IF(E15="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H15&amp;" by "&amp;IF(ISNA(VLOOKUP(C15,lookup!$A$2:$B$4,2,FALSE)=TRUE),C15,VLOOKUP(C15,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Hymenolepis nana by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O15" s="1" t="str">
         <f>IF($D15="count","a count of the number of ",IF($D15="boolean","a categorical measurement datum",IF($E15="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H15&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C15,lookup!$A$2:$B$4,2,FALSE)=TRUE),C15,VLOOKUP(C15,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B15&amp;" specimen")</f>
-        <v>a threshold cycle that is about Hymenolepis nana and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P15" s="1" t="str">
         <f>"("&amp;IF($D15="count","count and",IF($D15="boolean","'categorical measurement datum' and",IF($E15="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H15&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C15,lookup!$A$2:$B$4,2,FALSE)=TRUE),C15,VLOOKUP(C15,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B15&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Hymenolepis nana') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" t="s">
-        <v>70</v>
-      </c>
-      <c r="J16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Mycobacterium tuberculosis Ct value, by TAQ result</v>
-      </c>
-      <c r="K16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw bacteria data</v>
-      </c>
-      <c r="L16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="N16" s="1" t="str">
         <f>IF(D16="boolean","presence of",IF(D16="count","count of",IF(E16="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H16&amp;" by "&amp;IF(ISNA(VLOOKUP(C16,lookup!$A$2:$B$4,2,FALSE)=TRUE),C16,VLOOKUP(C16,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Mycobacterium tuberculosis by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O16" s="1" t="str">
         <f>IF($D16="count","a count of the number of ",IF($D16="boolean","a categorical measurement datum",IF($E16="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H16&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C16,lookup!$A$2:$B$4,2,FALSE)=TRUE),C16,VLOOKUP(C16,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B16&amp;" specimen")</f>
-        <v>a threshold cycle that is about Mycobacterium tuberculosis and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P16" s="1" t="str">
         <f>"("&amp;IF($D16="count","count and",IF($D16="boolean","'categorical measurement datum' and",IF($E16="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H16&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C16,lookup!$A$2:$B$4,2,FALSE)=TRUE),C16,VLOOKUP(C16,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B16&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Mycobacterium tuberculosis') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Norovirus GI 1 Ct value, by TAQ result</v>
-      </c>
-      <c r="K17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw virus data</v>
-      </c>
-      <c r="L17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="17" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N17" s="1" t="str">
         <f>IF(D17="boolean","presence of",IF(D17="count","count of",IF(E17="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H17&amp;" by "&amp;IF(ISNA(VLOOKUP(C17,lookup!$A$2:$B$4,2,FALSE)=TRUE),C17,VLOOKUP(C17,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Norovirus GI 1 by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O17" s="1" t="str">
         <f>IF($D17="count","a count of the number of ",IF($D17="boolean","a categorical measurement datum",IF($E17="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H17&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C17,lookup!$A$2:$B$4,2,FALSE)=TRUE),C17,VLOOKUP(C17,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B17&amp;" specimen")</f>
-        <v>a threshold cycle that is about Norovirus GI 1 and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P17" s="1" t="str">
         <f>"("&amp;IF($D17="count","count and",IF($D17="boolean","'categorical measurement datum' and",IF($E17="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H17&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C17,lookup!$A$2:$B$4,2,FALSE)=TRUE),C17,VLOOKUP(C17,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B17&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Norovirus GI 1') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" t="s">
-        <v>57</v>
-      </c>
-      <c r="H18" t="s">
-        <v>72</v>
-      </c>
-      <c r="J18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Norovirus GII 4 Ct value, by TAQ result</v>
-      </c>
-      <c r="K18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw virus data</v>
-      </c>
-      <c r="L18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="18" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N18" s="1" t="str">
         <f>IF(D18="boolean","presence of",IF(D18="count","count of",IF(E18="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H18&amp;" by "&amp;IF(ISNA(VLOOKUP(C18,lookup!$A$2:$B$4,2,FALSE)=TRUE),C18,VLOOKUP(C18,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Norovirus GII 4 by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O18" s="1" t="str">
         <f>IF($D18="count","a count of the number of ",IF($D18="boolean","a categorical measurement datum",IF($E18="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H18&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C18,lookup!$A$2:$B$4,2,FALSE)=TRUE),C18,VLOOKUP(C18,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B18&amp;" specimen")</f>
-        <v>a threshold cycle that is about Norovirus GII 4 and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P18" s="1" t="str">
         <f>"("&amp;IF($D18="count","count and",IF($D18="boolean","'categorical measurement datum' and",IF($E18="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H18&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C18,lookup!$A$2:$B$4,2,FALSE)=TRUE),C18,VLOOKUP(C18,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B18&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Norovirus GII 4') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Plesiomonas Ct value, by TAQ result</v>
-      </c>
-      <c r="K19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw bacteria data</v>
-      </c>
-      <c r="L19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="19" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N19" s="1" t="str">
         <f>IF(D19="boolean","presence of",IF(D19="count","count of",IF(E19="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H19&amp;" by "&amp;IF(ISNA(VLOOKUP(C19,lookup!$A$2:$B$4,2,FALSE)=TRUE),C19,VLOOKUP(C19,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Plesiomonas by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O19" s="1" t="str">
         <f>IF($D19="count","a count of the number of ",IF($D19="boolean","a categorical measurement datum",IF($E19="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H19&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C19,lookup!$A$2:$B$4,2,FALSE)=TRUE),C19,VLOOKUP(C19,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B19&amp;" specimen")</f>
-        <v>a threshold cycle that is about Plesiomonas and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P19" s="1" t="str">
         <f>"("&amp;IF($D19="count","count and",IF($D19="boolean","'categorical measurement datum' and",IF($E19="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H19&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C19,lookup!$A$2:$B$4,2,FALSE)=TRUE),C19,VLOOKUP(C19,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B19&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Plesiomonas') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" t="s">
-        <v>59</v>
-      </c>
-      <c r="J20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schistosoma Ct value, by TAQ result</v>
-      </c>
-      <c r="K20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw eukaryota data</v>
-      </c>
-      <c r="L20" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="20" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N20" s="1" t="str">
         <f>IF(D20="boolean","presence of",IF(D20="count","count of",IF(E20="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H20&amp;" by "&amp;IF(ISNA(VLOOKUP(C20,lookup!$A$2:$B$4,2,FALSE)=TRUE),C20,VLOOKUP(C20,lookup!$A$2:$B$4,2))</f>
-        <v>threshold cycle indicating Schistosoma by fluorogenic PCR assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O20" s="1" t="str">
         <f>IF($D20="count","a count of the number of ",IF($D20="boolean","a categorical measurement datum",IF($E20="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H20&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C20,lookup!$A$2:$B$4,2,FALSE)=TRUE),C20,VLOOKUP(C20,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B20&amp;" specimen")</f>
-        <v>a threshold cycle that is about Schistosoma and is the specified output of some fluorogenic PCR assay, which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P20" s="1" t="str">
         <f>"("&amp;IF($D20="count","count and",IF($D20="boolean","'categorical measurement datum' and",IF($E20="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H20&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C20,lookup!$A$2:$B$4,2,FALSE)=TRUE),C20,VLOOKUP(C20,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B20&amp;" specimen')"</f>
-        <v>('threshold cycle' and 'is about' some 'Schistosoma') and is_specified_output_of some (('fluorogenic PCR assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" t="s">
-        <v>76</v>
-      </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Aeromonas, by bacteriology result</v>
-      </c>
-      <c r="K21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Raw virus data</v>
-      </c>
-      <c r="L21" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Raw test result</v>
-      </c>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+      </c>
+    </row>
+    <row r="21" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N21" s="1" t="str">
         <f>IF(D21="boolean","presence of",IF(D21="count","count of",IF(E21="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H21&amp;" by "&amp;IF(ISNA(VLOOKUP(C21,lookup!$A$2:$B$4,2,FALSE)=TRUE),C21,VLOOKUP(C21,lookup!$A$2:$B$4,2))</f>
-        <v>data about Aeromonas by differential medium assay</v>
+        <v xml:space="preserve">data about  by </v>
       </c>
       <c r="O21" s="1" t="str">
         <f>IF($D21="count","a count of the number of ",IF($D21="boolean","a categorical measurement datum",IF($E21="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H21&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C21,lookup!$A$2:$B$4,2,FALSE)=TRUE),C21,VLOOKUP(C21,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B21&amp;" specimen")</f>
-        <v>a data item that is about Aeromonas and is the specified output of some differential medium assay, which achieves an organism identification objective and has as specified input a stool specimen</v>
+        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
       </c>
       <c r="P21" s="1" t="str">
         <f>"("&amp;IF($D21="count","count and",IF($D21="boolean","'categorical measurement datum' and",IF($E21="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H21&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C21,lookup!$A$2:$B$4,2,FALSE)=TRUE),C21,VLOOKUP(C21,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B21&amp;" specimen')"</f>
-        <v>('data item' and 'is about' some 'Aeromonas') and is_specified_output_of some (('differential medium assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
+        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
       </c>
     </row>
   </sheetData>
@@ -2085,19 +1593,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2130,7 +1638,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2138,13 +1646,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2155,21 +1663,21 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>"'fluorogenic PCR assay'"</f>

</xml_diff>

<commit_message>
fixed MALEDP3 subclass issue
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@100914 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D96C60E-F5B9-6244-AE04-2595CE470C1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB0177F-6BD5-C24B-A557-24DE309637CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>variable</t>
   </si>
@@ -211,6 +211,21 @@
   </si>
   <si>
     <t>stools</t>
+  </si>
+  <si>
+    <t>Norovirus GII.4</t>
+  </si>
+  <si>
+    <t>Norovirus</t>
+  </si>
+  <si>
+    <t>Chikungunya</t>
+  </si>
+  <si>
+    <t>OD cutoff value</t>
+  </si>
+  <si>
+    <t>SD Bioline IgM ELISA</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1073,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,7 +1268,7 @@
         <v>49</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f t="shared" ref="J4:J7" si="0">IF(ISNUMBER(SEARCH("stools",$E4)),"Cumulative sum ","")
+        <f t="shared" ref="J4:J9" si="0">IF(ISNUMBER(SEARCH("stools",$E4)),"Cumulative sum ","")
 &amp;$H4
 &amp;IF(ISNUMBER(SEARCH("stools",$E4)),"-pos ","")
 &amp;IF(ISNUMBER(SEARCH("1st monthly",$E4)),"1st monthly ","")
@@ -1266,7 +1281,7 @@
         <v>Adenovirus, by TAC result</v>
       </c>
       <c r="K4" s="1" t="str">
-        <f t="shared" ref="K4:K7" si="1">IF($D4="raw","Raw "&amp;LOWER($F4)&amp;" data ",
+        <f t="shared" ref="K4:K9" si="1">IF($D4="raw","Raw "&amp;LOWER($F4)&amp;" data ",
 IF($G4="",$H4,
 IF($D4="aggregate",$H4&amp;" aggregate data ",$G4)))
 &amp;IF(NOT(OR($D4="raw",ISNUMBER(SEARCH("stools",$E4)))),"in "&amp;$B4,"")</f>
@@ -1450,32 +1465,108 @@
         <v>('data item' and 'is about' some 'Campylobacter') and is_specified_output_of some (('ELISA' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Norovirus GII.4 Ct value, by TAC result</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Raw virus data </v>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f>IF(
+$D8="raw","Raw test result",
+$F8&amp;" "
+&amp;IF(NOT(ISNUMBER(SEARCH("stools",$E8))),"in "&amp;$B8&amp;" ","")
+)
+&amp;IF($D8="aggregate","detection aggregate data","")</f>
+        <v>Raw test result</v>
+      </c>
       <c r="N8" s="1" t="str">
         <f>IF(D8="boolean","presence of",IF(D8="count","count of",IF(E8="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H8&amp;" by "&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))</f>
-        <v xml:space="preserve">data about  by </v>
+        <v>threshold cycle indicating Norovirus GII.4 by TAC</v>
       </c>
       <c r="O8" s="1" t="str">
         <f>IF($D8="count","a count of the number of ",IF($D8="boolean","a categorical measurement datum",IF($E8="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H8&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B8&amp;" specimen")</f>
-        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a threshold cycle that is about Norovirus GII.4 and is the specified output of some TAC, which achieves an organism identification objective and has as specified input a stool specimen</v>
       </c>
       <c r="P8" s="1" t="str">
         <f>"("&amp;IF($D8="count","count and",IF($D8="boolean","'categorical measurement datum' and",IF($E8="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H8&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B8&amp;" specimen')"</f>
-        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>('threshold cycle' and 'is about' some 'Norovirus GII.4') and is_specified_output_of some (('TAC' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Chikungunya OD cutoff value, by SD Bioline IgM ELISA result</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Raw virus data </v>
+      </c>
+      <c r="L9" s="1" t="str">
+        <f>IF(
+$D9="raw","Raw test result",
+$F9&amp;" "
+&amp;IF(NOT(ISNUMBER(SEARCH("stools",$E9))),"in "&amp;$B9&amp;" ","")
+)
+&amp;IF($D9="aggregate","detection aggregate data","")</f>
+        <v>Raw test result</v>
+      </c>
       <c r="N9" s="1" t="str">
         <f>IF(D9="boolean","presence of",IF(D9="count","count of",IF(E9="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H9&amp;" by "&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))</f>
-        <v xml:space="preserve">data about  by </v>
+        <v>data about Chikungunya by SD Bioline IgM ELISA</v>
       </c>
       <c r="O9" s="1" t="str">
         <f>IF($D9="count","a count of the number of ",IF($D9="boolean","a categorical measurement datum",IF($E9="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H9&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B9&amp;" specimen")</f>
-        <v>a data item that is about  and is the specified output of some , which achieves an organism identification objective and has as specified input a  specimen</v>
+        <v>a data item that is about Chikungunya and is the specified output of some SD Bioline IgM ELISA, which achieves an organism identification objective and has as specified input a stool specimen</v>
       </c>
       <c r="P9" s="1" t="str">
         <f>"("&amp;IF($D9="count","count and",IF($D9="boolean","'categorical measurement datum' and",IF($E9="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H9&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B9&amp;" specimen')"</f>
-        <v>('data item' and 'is about' some '') and is_specified_output_of some (('' and achieves_planned_objective some 'organism identification objective') and has_specified_input some ' specimen')</v>
+        <v>('data item' and 'is about' some 'Chikungunya') and is_specified_output_of some (('SD Bioline IgM ELISA' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
rebuilt MALEDp3 conversion file
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@100958 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/script/detection_template.xlsx
+++ b/Load/ontology/script/detection_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A35D5C-336B-004C-8411-943C2AEE6E3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2D1FFE-A1AA-B146-89C0-808D5A696795}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="33600" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="detection_template_csv" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t>variable</t>
   </si>
@@ -72,9 +72,6 @@
     <t>input "Bacteria", "Eukaryota", or "Virus"</t>
   </si>
   <si>
-    <t>First, either enter genus and species, or E. coli type abbrev. (e.g. ETEC). Then, enter any additional specifics from data provider (serotype, gene).</t>
-  </si>
-  <si>
     <t>&lt;--INPUT | OUTPUT --&gt;</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Parent term in ClinEpi (which genus in which sample type)</t>
   </si>
   <si>
-    <t>(which domain in which sample type)</t>
-  </si>
-  <si>
     <t>axiom</t>
   </si>
   <si>
@@ -226,13 +220,94 @@
   </si>
   <si>
     <t>1st diarrheal stools</t>
+  </si>
+  <si>
+    <t>Vibrio cholerae Ct value, by microscopy result</t>
+  </si>
+  <si>
+    <t>Adenovirus, by TAC result</t>
+  </si>
+  <si>
+    <t>Aeromonas Ct value, by TAC result</t>
+  </si>
+  <si>
+    <t>Ancylostoma Ct value, by TAC result</t>
+  </si>
+  <si>
+    <t>Cumulative sum Campylobacter-pos 1st diarrheal stools, by ELISA</t>
+  </si>
+  <si>
+    <t>Norovirus GII.4 Ct value, by TAC result</t>
+  </si>
+  <si>
+    <t>Chikungunya OD cutoff value, by SD Bioline IgM ELISA result</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">First, either enter genus and species, or </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>E. coli type abbrev. (e.g. ETEC)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Then, enter any additional specifics from data provider (serotype, gene).</t>
+    </r>
+  </si>
+  <si>
+    <t>E.g. Enteroaggressive, Shigatoxin producing</t>
+  </si>
+  <si>
+    <t>Escherichia</t>
+  </si>
+  <si>
+    <t>Enteroaggressive</t>
+  </si>
+  <si>
+    <t>enterotoxin or virulence factor 1</t>
+  </si>
+  <si>
+    <t>enterotoxin or virulence factor 2</t>
+  </si>
+  <si>
+    <t>aaiC</t>
+  </si>
+  <si>
+    <t>aatA</t>
+  </si>
+  <si>
+    <t>If one of the factors is negative, which one?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -366,6 +441,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1070,13 +1151,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
@@ -1086,17 +1170,18 @@
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="34.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="74.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="187.83203125" customWidth="1"/>
-    <col min="16" max="16" width="214.5" customWidth="1"/>
+    <col min="9" max="12" width="24.83203125" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="45.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="34.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="74.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="187.83203125" customWidth="1"/>
+    <col min="20" max="20" width="214.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="34">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -1121,43 +1206,52 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="T1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="102">
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -1166,47 +1260,47 @@
         <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="125" customHeight="1">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="1" t="str">
+      <c r="N3" s="1" t="str">
         <f>IF(ISNUMBER(SEARCH("stools",$E3)),"Cumulative sum ","")
 &amp;$H3
 &amp;IF(ISNUMBER(SEARCH("stools",$E3)),"-pos ","")
@@ -1219,15 +1313,15 @@
 &amp;IF($D3="raw"," result","")</f>
         <v>Vibrio cholerae Ct value, by microscopy result</v>
       </c>
-      <c r="K3" s="1" t="str">
+      <c r="O3" s="1" t="str">
         <f>IF($D3="raw","Raw "&amp;LOWER($F3)&amp;" data ",
 IF($G3="",$H3,
 IF($D3="aggregate",$H3&amp;" aggregate data ",$G3)))
 &amp;IF(NOT(OR($D3="raw",ISNUMBER(SEARCH("stools",$E3)))),"in "&amp;$B3,"")</f>
         <v xml:space="preserve">Raw bacteria data </v>
       </c>
-      <c r="L3" s="1" t="str">
-        <f t="shared" ref="L3:L9" si="0">IF(
+      <c r="P3" s="1" t="str">
+        <f t="shared" ref="P3:P10" si="0">IF(
 $D3="raw","Raw test result",
 $F3&amp;" "
 &amp;IF(NOT(ISNUMBER(SEARCH("stools",$E3))),"in "&amp;$B3&amp;" ","")
@@ -1235,40 +1329,40 @@
 &amp;IF($D3="aggregate","detection aggregate data","")</f>
         <v>Raw test result</v>
       </c>
-      <c r="N3" s="1" t="str">
+      <c r="R3" s="1" t="str">
         <f>IF(D3="boolean","presence of",IF(D3="count","count of",IF(E3="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H3&amp;" by "&amp;IF(ISNA(VLOOKUP(C3,lookup!$A$2:$B$4,2,FALSE)=TRUE),C3,VLOOKUP(C3,lookup!$A$2:$B$4,2))</f>
         <v>threshold cycle indicating Vibrio cholerae by microscopy</v>
       </c>
-      <c r="O3" s="1" t="str">
+      <c r="S3" s="1" t="str">
         <f>IF($D3="count","a count of the number of ",IF($D3="boolean","a categorical measurement datum",IF($E3="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H3&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C3,lookup!$A$2:$B$4,2,FALSE)=TRUE),C3,VLOOKUP(C3,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B3&amp;" specimen")</f>
         <v>a threshold cycle that is about Vibrio cholerae and is the specified output of some microscopy, which achieves an organism identification objective and has as specified input a stool specimen</v>
       </c>
-      <c r="P3" s="1" t="str">
+      <c r="T3" s="1" t="str">
         <f>"("&amp;IF($D3="count","count and",IF($D3="boolean","'categorical measurement datum' and",IF($E3="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H3&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C3,lookup!$A$2:$B$4,2,FALSE)=TRUE),C3,VLOOKUP(C3,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B3&amp;" specimen')"</f>
         <v>('threshold cycle' and 'is about' some 'Vibrio cholerae') and is_specified_output_of some (('microscopy' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="42" customHeight="1">
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f t="shared" ref="J4:J9" si="1">IF(ISNUMBER(SEARCH("stools",$E4)),"Cumulative sum ","")
+      <c r="N4" s="1" t="str">
+        <f t="shared" ref="N4:N10" si="1">IF(ISNUMBER(SEARCH("stools",$E4)),"Cumulative sum ","")
 &amp;$H4
 &amp;IF(ISNUMBER(SEARCH("stools",$E4)),"-pos ","")
 &amp;IF(ISNUMBER(SEARCH("1st monthly",$E4)),"1st monthly ","")
@@ -1280,312 +1374,429 @@
 &amp;IF($D4="raw"," result","")</f>
         <v>Adenovirus, by TAC result</v>
       </c>
-      <c r="K4" s="1" t="str">
-        <f t="shared" ref="K4:K9" si="2">IF($D4="raw","Raw "&amp;LOWER($F4)&amp;" data ",
+      <c r="O4" s="1" t="str">
+        <f t="shared" ref="O4:O10" si="2">IF($D4="raw","Raw "&amp;LOWER($F4)&amp;" data ",
 IF($G4="",$H4,
 IF($D4="aggregate",$H4&amp;" aggregate data ",$G4)))
 &amp;IF(NOT(OR($D4="raw",ISNUMBER(SEARCH("stools",$E4)))),"in "&amp;$B4,"")</f>
         <v xml:space="preserve">Raw virus data </v>
       </c>
-      <c r="L4" s="1" t="str">
+      <c r="P4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Raw test result</v>
       </c>
-      <c r="N4" s="1" t="str">
+      <c r="R4" s="1" t="str">
         <f>IF(D4="boolean","presence of",IF(D4="count","count of",IF(E4="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H4&amp;" by "&amp;IF(ISNA(VLOOKUP(C4,lookup!$A$2:$B$4,2,FALSE)=TRUE),C4,VLOOKUP(C4,lookup!$A$2:$B$4,2))</f>
         <v>data about Adenovirus by TAC</v>
       </c>
-      <c r="O4" s="1" t="str">
+      <c r="S4" s="1" t="str">
         <f>IF($D4="count","a count of the number of ",IF($D4="boolean","a categorical measurement datum",IF($E4="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H4&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C4,lookup!$A$2:$B$4,2,FALSE)=TRUE),C4,VLOOKUP(C4,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B4&amp;" specimen")</f>
         <v>a data item that is about Adenovirus and is the specified output of some TAC, which achieves an organism identification objective and has as specified input a urine specimen</v>
       </c>
-      <c r="P4" s="1" t="str">
+      <c r="T4" s="1" t="str">
         <f>"("&amp;IF($D4="count","count and",IF($D4="boolean","'categorical measurement datum' and",IF($E4="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H4&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C4,lookup!$A$2:$B$4,2,FALSE)=TRUE),C4,VLOOKUP(C4,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B4&amp;" specimen')"</f>
         <v>('data item' and 'is about' some 'Adenovirus') and is_specified_output_of some (('TAC' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'urine specimen')</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="17">
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="1" t="str">
+        <v>48</v>
+      </c>
+      <c r="N5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aeromonas Ct value, by TAC result</v>
       </c>
-      <c r="K5" s="1" t="str">
+      <c r="O5" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">Raw virus data </v>
       </c>
-      <c r="L5" s="1" t="str">
+      <c r="P5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Raw test result</v>
       </c>
-      <c r="N5" s="1" t="str">
+      <c r="R5" s="1" t="str">
         <f>IF(D5="boolean","presence of",IF(D5="count","count of",IF(E5="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H5&amp;" by "&amp;IF(ISNA(VLOOKUP(C5,lookup!$A$2:$B$4,2,FALSE)=TRUE),C5,VLOOKUP(C5,lookup!$A$2:$B$4,2))</f>
         <v>threshold cycle indicating Aeromonas by TAC</v>
       </c>
-      <c r="O5" s="1" t="str">
+      <c r="S5" s="1" t="str">
         <f>IF($D5="count","a count of the number of ",IF($D5="boolean","a categorical measurement datum",IF($E5="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H5&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C5,lookup!$A$2:$B$4,2,FALSE)=TRUE),C5,VLOOKUP(C5,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B5&amp;" specimen")</f>
         <v>a threshold cycle that is about Aeromonas and is the specified output of some TAC, which achieves an organism identification objective and has as specified input a urine specimen</v>
       </c>
-      <c r="P5" s="1" t="str">
+      <c r="T5" s="1" t="str">
         <f>"("&amp;IF($D5="count","count and",IF($D5="boolean","'categorical measurement datum' and",IF($E5="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H5&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C5,lookup!$A$2:$B$4,2,FALSE)=TRUE),C5,VLOOKUP(C5,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B5&amp;" specimen')"</f>
         <v>('threshold cycle' and 'is about' some 'Aeromonas') and is_specified_output_of some (('TAC' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'urine specimen')</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="17">
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="1" t="str">
+        <v>49</v>
+      </c>
+      <c r="N6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Ancylostoma Ct value, by TAC result</v>
       </c>
-      <c r="K6" s="1" t="str">
+      <c r="O6" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">Raw eukaryota data </v>
       </c>
-      <c r="L6" s="1" t="str">
+      <c r="P6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Raw test result</v>
       </c>
-      <c r="N6" s="1" t="str">
+      <c r="R6" s="1" t="str">
         <f>IF(D6="boolean","presence of",IF(D6="count","count of",IF(E6="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H6&amp;" by "&amp;IF(ISNA(VLOOKUP(C6,lookup!$A$2:$B$4,2,FALSE)=TRUE),C6,VLOOKUP(C6,lookup!$A$2:$B$4,2))</f>
         <v>threshold cycle indicating Ancylostoma by TAC</v>
       </c>
-      <c r="O6" s="1" t="str">
+      <c r="S6" s="1" t="str">
         <f>IF($D6="count","a count of the number of ",IF($D6="boolean","a categorical measurement datum",IF($E6="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H6&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C6,lookup!$A$2:$B$4,2,FALSE)=TRUE),C6,VLOOKUP(C6,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B6&amp;" specimen")</f>
         <v>a threshold cycle that is about Ancylostoma and is the specified output of some TAC, which achieves an organism identification objective and has as specified input a urine specimen</v>
       </c>
-      <c r="P6" s="1" t="str">
+      <c r="T6" s="1" t="str">
         <f>"("&amp;IF($D6="count","count and",IF($D6="boolean","'categorical measurement datum' and",IF($E6="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H6&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C6,lookup!$A$2:$B$4,2,FALSE)=TRUE),C6,VLOOKUP(C6,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B6&amp;" specimen')"</f>
         <v>('threshold cycle' and 'is about' some 'Ancylostoma') and is_specified_output_of some (('TAC' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'urine specimen')</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="94" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="94" customHeight="1">
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="1" t="str">
+        <v>57</v>
+      </c>
+      <c r="N7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Cumulative sum Campylobacter-pos 1st diarrheal stools, by ELISA</v>
       </c>
-      <c r="K7" s="1" t="str">
+      <c r="O7" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">Campylobacter aggregate data </v>
       </c>
-      <c r="L7" s="1" t="str">
+      <c r="P7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Bacteria detection aggregate data</v>
       </c>
-      <c r="N7" s="1" t="str">
+      <c r="R7" s="1" t="str">
         <f>IF(D7="boolean","presence of",IF(D7="count","count of",IF(E7="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H7&amp;" by "&amp;IF(ISNA(VLOOKUP(C7,lookup!$A$2:$B$4,2,FALSE)=TRUE),C7,VLOOKUP(C7,lookup!$A$2:$B$4,2))</f>
         <v>data about Campylobacter by ELISA</v>
       </c>
-      <c r="O7" s="1" t="str">
+      <c r="S7" s="1" t="str">
         <f>IF($D7="count","a count of the number of ",IF($D7="boolean","a categorical measurement datum",IF($E7="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H7&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C7,lookup!$A$2:$B$4,2,FALSE)=TRUE),C7,VLOOKUP(C7,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B7&amp;" specimen")</f>
         <v>a data item that is about Campylobacter and is the specified output of some ELISA, which achieves an organism identification objective and has as specified input a stool specimen</v>
       </c>
-      <c r="P7" s="1" t="str">
+      <c r="T7" s="1" t="str">
         <f>"("&amp;IF($D7="count","count and",IF($D7="boolean","'categorical measurement datum' and",IF($E7="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H7&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C7,lookup!$A$2:$B$4,2,FALSE)=TRUE),C7,VLOOKUP(C7,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B7&amp;" specimen')"</f>
         <v>('data item' and 'is about' some 'Campylobacter') and is_specified_output_of some (('ELISA' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="17">
       <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="N8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Norovirus GII.4 Ct value, by TAC result</v>
       </c>
-      <c r="K8" s="1" t="str">
+      <c r="O8" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">Raw virus data </v>
       </c>
-      <c r="L8" s="1" t="str">
+      <c r="P8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Raw test result</v>
       </c>
-      <c r="N8" s="1" t="str">
+      <c r="R8" s="1" t="str">
         <f>IF(D8="boolean","presence of",IF(D8="count","count of",IF(E8="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H8&amp;" by "&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))</f>
         <v>threshold cycle indicating Norovirus GII.4 by TAC</v>
       </c>
-      <c r="O8" s="1" t="str">
+      <c r="S8" s="1" t="str">
         <f>IF($D8="count","a count of the number of ",IF($D8="boolean","a categorical measurement datum",IF($E8="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H8&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B8&amp;" specimen")</f>
         <v>a threshold cycle that is about Norovirus GII.4 and is the specified output of some TAC, which achieves an organism identification objective and has as specified input a stool specimen</v>
       </c>
-      <c r="P8" s="1" t="str">
+      <c r="T8" s="1" t="str">
         <f>"("&amp;IF($D8="count","count and",IF($D8="boolean","'categorical measurement datum' and",IF($E8="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H8&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C8,lookup!$A$2:$B$4,2,FALSE)=TRUE),C8,VLOOKUP(C8,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B8&amp;" specimen')"</f>
         <v>('threshold cycle' and 'is about' some 'Norovirus GII.4') and is_specified_output_of some (('TAC' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="34">
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="N9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Chikungunya OD cutoff value, by SD Bioline IgM ELISA result</v>
       </c>
-      <c r="K9" s="1" t="str">
+      <c r="O9" s="1" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">Raw virus data </v>
       </c>
-      <c r="L9" s="1" t="str">
+      <c r="P9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Raw test result</v>
       </c>
-      <c r="N9" s="1" t="str">
+      <c r="R9" s="1" t="str">
         <f>IF(D9="boolean","presence of",IF(D9="count","count of",IF(E9="Ct value","threshold cycle indicating","data about")))&amp;" "&amp;H9&amp;" by "&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))</f>
         <v>data about Chikungunya by SD Bioline IgM ELISA</v>
       </c>
-      <c r="O9" s="1" t="str">
+      <c r="S9" s="1" t="str">
         <f>IF($D9="count","a count of the number of ",IF($D9="boolean","a categorical measurement datum",IF($E9="Ct value","a threshold cycle","a data item")&amp;" that is about ")&amp;$H9&amp;" and is the specified output of some "&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))&amp;", which achieves an organism identification objective and has as specified input a "&amp;$B9&amp;" specimen")</f>
         <v>a data item that is about Chikungunya and is the specified output of some SD Bioline IgM ELISA, which achieves an organism identification objective and has as specified input a stool specimen</v>
       </c>
-      <c r="P9" s="1" t="str">
+      <c r="T9" s="1" t="str">
         <f>"("&amp;IF($D9="count","count and",IF($D9="boolean","'categorical measurement datum' and",IF($E9="Ct value","'threshold cycle' and","'data item' and"))&amp;" 'is about' some ")&amp;"'"&amp;$H9&amp;"') and is_specified_output_of some (('"&amp;IF(ISNA(VLOOKUP(C9,lookup!$A$2:$B$4,2,FALSE)=TRUE),C9,VLOOKUP(C9,lookup!$A$2:$B$4,2))&amp;"' and achieves_planned_objective some 'organism identification objective') and has_specified_input some '"&amp;$B9&amp;" specimen')"</f>
         <v>('data item' and 'is about' some 'Chikungunya') and is_specified_output_of some (('SD Bioline IgM ELISA' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'stool specimen')</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+    <row r="10" spans="1:20" ht="34">
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Cumulative sum Escherichia coli-pos 1st diarrheal stools</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">Escherichia coli aggregate data </v>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Bacteria detection aggregate data</v>
+      </c>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" ht="17">
+      <c r="N12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" ht="17">
+      <c r="N13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" ht="17">
+      <c r="N14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" ht="17">
+      <c r="N15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" ht="34">
+      <c r="N16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="14:20" ht="17">
+      <c r="N17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="14:20" ht="34">
+      <c r="N18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="14:20">
+      <c r="P19" s="1" t="str">
+        <f>IF(ISNUMBER(SEARCH("stools",$E19)),"Cumulative sum ","")
+&amp;$H19
+&amp;IF(ISNUMBER(SEARCH("stools",$E19)),"-pos ","")
+&amp;IF(ISNUMBER(SEARCH("1st monthly",$E19)),"1st monthly ","")
+&amp;IF(ISNUMBER(SEARCH("1st diarrheal",$E19)),"1st diarrheal ","")
+&amp;IF(ISNUMBER(SEARCH("stools",$E19)),"stools","")
+&amp;IF($D19="raw",IF($E19&lt;&gt;""," ","")&amp;$E19,"")
+&amp;IF($D19="count"," count","")
+&amp;IF($C19&lt;&gt;"",", by "&amp;$C19,"")
+&amp;IF($D19="raw"," result","")</f>
+        <v/>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="14:20">
+      <c r="P20" s="1" t="str">
+        <f t="shared" ref="P20:P25" si="3">IF(ISNUMBER(SEARCH("stools",$E20)),"Cumulative sum ","")
+&amp;$H20
+&amp;IF(ISNUMBER(SEARCH("stools",$E20)),"-pos ","")
+&amp;IF(ISNUMBER(SEARCH("1st monthly",$E20)),"1st monthly ","")
+&amp;IF(ISNUMBER(SEARCH("1st diarrheal",$E20)),"1st diarrheal ","")
+&amp;IF(ISNUMBER(SEARCH("stools",$E20)),"stools","")
+&amp;IF($D20="raw",IF($E20&lt;&gt;""," ","")&amp;$E20,"")
+&amp;IF($D20="count"," count","")
+&amp;IF($C20&lt;&gt;"",", by "&amp;$C20,"")
+&amp;IF($D20="raw"," result","")</f>
+        <v/>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="14:20">
+      <c r="P21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="14:20">
+      <c r="P22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="14:20">
+      <c r="P23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="14:20">
+      <c r="P24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="14:20">
+      <c r="P25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1601,27 +1812,27 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1637,13 +1848,13 @@
       <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1654,24 +1865,24 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1679,21 +1890,21 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>"'fluorogenic PCR assay'"</f>

</xml_diff>